<commit_message>
updated problem 3.8 writeup, added 3 png graphs for it, 1 layer 80, and 2 layer graphs
</commit_message>
<xml_diff>
--- a/michael-part/Hidden 30 Raw Perf Data.xlsx
+++ b/michael-part/Hidden 30 Raw Perf Data.xlsx
@@ -4,19 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hidden 0.1" sheetId="1" r:id="rId1"/>
     <sheet name="Hidden 0.01" sheetId="2" r:id="rId2"/>
     <sheet name="Hidden 1.0" sheetId="3" r:id="rId3"/>
     <sheet name="Hiden 0.001" sheetId="4" r:id="rId4"/>
+    <sheet name="80 units" sheetId="5" r:id="rId5"/>
+    <sheet name="2 layer 10 total" sheetId="6" r:id="rId6"/>
+    <sheet name="2 layer 30 total" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="hidden2l10" localSheetId="5">'2 layer 10 total'!$B$3:$J$107</definedName>
+    <definedName name="hidden2l30" localSheetId="6">'2 layer 30 total'!$B$4:$J$79</definedName>
     <definedName name="hidden30lr001" localSheetId="3">'Hiden 0.001'!$B$3:$J$90</definedName>
     <definedName name="hidden30lr01" localSheetId="1">'Hidden 0.01'!$B$4:$F$86</definedName>
     <definedName name="hidden30lr1" localSheetId="0">'Hidden 0.1'!$C$3:$G$85</definedName>
     <definedName name="hidden30lrone" localSheetId="2">'Hidden 1.0'!$B$3:$J$89</definedName>
+    <definedName name="hidden80" localSheetId="4">'80 units'!$B$4:$J$23</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +35,37 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="hidden30lr001.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="hidden2l10.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:michael-part:hidden2l10.txt" space="1" consecutive="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="hidden2l30.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:michael-part:hidden2l30.txt" space="1" consecutive="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="hidden30lr001.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:hidden30lr001.txt" space="1" consecutive="1">
       <textFields count="9">
         <textField/>
@@ -44,7 +80,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="hidden30lr01.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="hidden30lr01.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="6" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:hidden30lr01.txt" space="1" consecutive="1">
       <textFields count="5">
         <textField/>
@@ -55,8 +91,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="hidden30lr1.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="6" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:hidden30lr1.txt" space="1" consecutive="1">
+  <connection id="5" name="hidden30lr1.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="6" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:hidden30lr1.txt" space="1" consecutive="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -66,8 +102,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="hidden30lrone.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="hidden30lrone.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:hidden30lrone.txt" space="1" consecutive="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="hidden80.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Feynman:Users:michael:Documents:Harvard:CS 181:hw:hw2:michael-part:hidden80.txt" space="1" consecutive="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -85,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="28">
   <si>
     <t>Performance:</t>
   </si>
@@ -161,6 +212,15 @@
   <si>
     <t>Output</t>
   </si>
+  <si>
+    <t>80,</t>
+  </si>
+  <si>
+    <t>CustomNetwork</t>
+  </si>
+  <si>
+    <t>10,</t>
+  </si>
 </sst>
 </file>
 
@@ -208,8 +268,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -224,17 +290,23 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1103,11 +1175,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2144431592"/>
-        <c:axId val="2144429352"/>
+        <c:axId val="-2129646872"/>
+        <c:axId val="-2129649864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2144431592"/>
+        <c:axId val="-2129646872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1188,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144429352"/>
+        <c:crossAx val="-2129649864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1124,7 +1196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144429352"/>
+        <c:axId val="-2129649864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,14 +1207,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144431592"/>
+        <c:crossAx val="-2129646872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1193,19 +1264,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lr1" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lr1" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lr01" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lr01" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lrone" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lrone" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lr001" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden30lr001" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden80" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden2l10" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hidden2l30" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6982,7 +7065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -8546,4 +8629,3643 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.37288888999999997</v>
+      </c>
+      <c r="E9">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="F9">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.79444444000000003</v>
+      </c>
+      <c r="E10">
+        <v>0.76</v>
+      </c>
+      <c r="F10">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.85311110999999995</v>
+      </c>
+      <c r="E11">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="F11">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.87411110999999997</v>
+      </c>
+      <c r="E12">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.89288889000000005</v>
+      </c>
+      <c r="E14">
+        <v>0.873</v>
+      </c>
+      <c r="F14">
+        <v>0.92100000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="E15">
+        <v>0.88</v>
+      </c>
+      <c r="F15">
+        <v>0.92600000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.90488888999999995</v>
+      </c>
+      <c r="E16">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="F16">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.91</v>
+      </c>
+      <c r="E17">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="F17">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="E18">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F18">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.91788888999999996</v>
+      </c>
+      <c r="E19">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="F19">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0.92077777999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="F20">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0.92344444000000003</v>
+      </c>
+      <c r="E21">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="F21">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.92466667000000002</v>
+      </c>
+      <c r="E22">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="F22">
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.92733332999999996</v>
+      </c>
+      <c r="E23">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="F23">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J107"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:F107"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.10133333</v>
+      </c>
+      <c r="E8">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.105</v>
+      </c>
+      <c r="F9">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.105</v>
+      </c>
+      <c r="F10">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.105</v>
+      </c>
+      <c r="F11">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.105</v>
+      </c>
+      <c r="F12">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.105</v>
+      </c>
+      <c r="F13">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.105</v>
+      </c>
+      <c r="F14">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.105</v>
+      </c>
+      <c r="F15">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.105</v>
+      </c>
+      <c r="F16">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.105</v>
+      </c>
+      <c r="F17">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.105</v>
+      </c>
+      <c r="F18">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.105</v>
+      </c>
+      <c r="F19">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.105</v>
+      </c>
+      <c r="F20">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.105</v>
+      </c>
+      <c r="F21">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.105</v>
+      </c>
+      <c r="F22">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.105</v>
+      </c>
+      <c r="F23">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.105</v>
+      </c>
+      <c r="F24">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E25">
+        <v>0.105</v>
+      </c>
+      <c r="F25">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.105</v>
+      </c>
+      <c r="F26">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.105</v>
+      </c>
+      <c r="F27">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.105</v>
+      </c>
+      <c r="F28">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E29">
+        <v>0.105</v>
+      </c>
+      <c r="F29">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.105</v>
+      </c>
+      <c r="F30">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.105</v>
+      </c>
+      <c r="F31">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E32">
+        <v>0.105</v>
+      </c>
+      <c r="F32">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0.20077777999999999</v>
+      </c>
+      <c r="E33">
+        <v>0.191</v>
+      </c>
+      <c r="F33">
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0.21222221999999999</v>
+      </c>
+      <c r="E34">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0.21288889</v>
+      </c>
+      <c r="E35">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F35">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.21977778000000001</v>
+      </c>
+      <c r="E36">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F36">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0.27566667</v>
+      </c>
+      <c r="E37">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="F37">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0.31077778</v>
+      </c>
+      <c r="E38">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="F38">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0.32633332999999998</v>
+      </c>
+      <c r="E39">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F39">
+        <v>0.316</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="E40">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="F40">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0.32677778000000002</v>
+      </c>
+      <c r="E41">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="F41">
+        <v>0.316</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0.32488888999999999</v>
+      </c>
+      <c r="E42">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="F42">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43">
+        <v>36</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0.32611110999999998</v>
+      </c>
+      <c r="E43">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F43">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.33022222000000001</v>
+      </c>
+      <c r="E44">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="F44">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.33388888999999999</v>
+      </c>
+      <c r="E45">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="F45">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0.34</v>
+      </c>
+      <c r="E46">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="F46">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0.35044444000000002</v>
+      </c>
+      <c r="E47">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="F47">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0.35644443999999997</v>
+      </c>
+      <c r="E48">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="F48">
+        <v>0.372</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49">
+        <v>42</v>
+      </c>
+      <c r="C49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0.42655556</v>
+      </c>
+      <c r="E49">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="F49">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50">
+        <v>43</v>
+      </c>
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0.50188889000000003</v>
+      </c>
+      <c r="E50">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="F50">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51">
+        <v>44</v>
+      </c>
+      <c r="C51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0.55522221999999999</v>
+      </c>
+      <c r="E51">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F51">
+        <v>0.58799999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52">
+        <v>45</v>
+      </c>
+      <c r="C52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0.57833332999999998</v>
+      </c>
+      <c r="E52">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F52">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53">
+        <v>46</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.59488889</v>
+      </c>
+      <c r="E53">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="F53">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54">
+        <v>47</v>
+      </c>
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0.60144443999999997</v>
+      </c>
+      <c r="E54">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F54">
+        <v>0.61299999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0.60488889000000001</v>
+      </c>
+      <c r="E55">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="F55">
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56">
+        <v>49</v>
+      </c>
+      <c r="C56" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0.60744443999999997</v>
+      </c>
+      <c r="E56">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F56">
+        <v>0.626</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57">
+        <v>50</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0.60733333</v>
+      </c>
+      <c r="E57">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="F57">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58">
+        <v>51</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0.60466666999999996</v>
+      </c>
+      <c r="E58">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F58">
+        <v>0.628</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59">
+        <v>52</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0.60288889000000001</v>
+      </c>
+      <c r="E59">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="F59">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60">
+        <v>53</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0.60622222000000003</v>
+      </c>
+      <c r="E60">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="F60">
+        <v>0.63200000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="B61">
+        <v>54</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0.61033333000000001</v>
+      </c>
+      <c r="E61">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="F61">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62">
+        <v>55</v>
+      </c>
+      <c r="C62" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0.61433333000000001</v>
+      </c>
+      <c r="E62">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="F62">
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63">
+        <v>56</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0.61733333000000001</v>
+      </c>
+      <c r="E63">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="F63">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64">
+        <v>57</v>
+      </c>
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0.61888889000000002</v>
+      </c>
+      <c r="E64">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="F64">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65">
+        <v>58</v>
+      </c>
+      <c r="C65" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0.62055556000000001</v>
+      </c>
+      <c r="E65">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="F65">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66">
+        <v>59</v>
+      </c>
+      <c r="C66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0.62277777999999995</v>
+      </c>
+      <c r="E66">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="F66">
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67">
+        <v>60</v>
+      </c>
+      <c r="C67" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0.62466666999999998</v>
+      </c>
+      <c r="E67">
+        <v>0.59</v>
+      </c>
+      <c r="F67">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68">
+        <v>61</v>
+      </c>
+      <c r="C68" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0.625</v>
+      </c>
+      <c r="E68">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="F68">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69">
+        <v>62</v>
+      </c>
+      <c r="C69" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0.62711110999999997</v>
+      </c>
+      <c r="E69">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="F69">
+        <v>0.65300000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70">
+        <v>63</v>
+      </c>
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0.62977777999999995</v>
+      </c>
+      <c r="E70">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="F70">
+        <v>0.66100000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71">
+        <v>64</v>
+      </c>
+      <c r="C71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0.63322221999999995</v>
+      </c>
+      <c r="E71">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="F71">
+        <v>0.66800000000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72">
+        <v>65</v>
+      </c>
+      <c r="C72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0.63622221999999995</v>
+      </c>
+      <c r="E72">
+        <v>0.6</v>
+      </c>
+      <c r="F72">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73">
+        <v>66</v>
+      </c>
+      <c r="C73" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0.63977777999999996</v>
+      </c>
+      <c r="E73">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="F73">
+        <v>0.67300000000000004</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74">
+        <v>67</v>
+      </c>
+      <c r="C74" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.64311110999999999</v>
+      </c>
+      <c r="E74">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="F74">
+        <v>0.67300000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75">
+        <v>68</v>
+      </c>
+      <c r="C75" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0.64877777999999997</v>
+      </c>
+      <c r="E75">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="F75">
+        <v>0.67700000000000005</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76">
+        <v>69</v>
+      </c>
+      <c r="C76" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0.65577777999999998</v>
+      </c>
+      <c r="E76">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="F76">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77">
+        <v>70</v>
+      </c>
+      <c r="C77" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0.67344444000000003</v>
+      </c>
+      <c r="E77">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="F77">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78">
+        <v>71</v>
+      </c>
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0.70077778000000002</v>
+      </c>
+      <c r="E78">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="F78">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="B79">
+        <v>72</v>
+      </c>
+      <c r="C79" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0.71444443999999996</v>
+      </c>
+      <c r="E79">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="F79">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="B80">
+        <v>73</v>
+      </c>
+      <c r="C80" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0.72666666999999996</v>
+      </c>
+      <c r="E80">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="F80">
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81">
+        <v>74</v>
+      </c>
+      <c r="C81" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0.73333333000000001</v>
+      </c>
+      <c r="E81">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="F81">
+        <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82">
+        <v>75</v>
+      </c>
+      <c r="C82" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0.73477778000000005</v>
+      </c>
+      <c r="E82">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="F82">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83">
+        <v>76</v>
+      </c>
+      <c r="C83" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0.73833333000000001</v>
+      </c>
+      <c r="E83">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="F83">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84">
+        <v>77</v>
+      </c>
+      <c r="C84" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0.73577778000000005</v>
+      </c>
+      <c r="E84">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="F84">
+        <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6">
+      <c r="B85">
+        <v>78</v>
+      </c>
+      <c r="C85" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0.73844443999999998</v>
+      </c>
+      <c r="E85">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="F85">
+        <v>0.747</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="B86">
+        <v>79</v>
+      </c>
+      <c r="C86" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0.73711110999999996</v>
+      </c>
+      <c r="E86">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F86">
+        <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6">
+      <c r="B87">
+        <v>80</v>
+      </c>
+      <c r="C87" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0.73811110999999996</v>
+      </c>
+      <c r="E87">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="F87">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="B88">
+        <v>81</v>
+      </c>
+      <c r="C88" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="E88">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="F88">
+        <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6">
+      <c r="B89">
+        <v>82</v>
+      </c>
+      <c r="C89" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0.74</v>
+      </c>
+      <c r="E89">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="F89">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6">
+      <c r="B90">
+        <v>83</v>
+      </c>
+      <c r="C90" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0.74311110999999996</v>
+      </c>
+      <c r="E90">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="F90">
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6">
+      <c r="B91">
+        <v>84</v>
+      </c>
+      <c r="C91" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0.74688889000000003</v>
+      </c>
+      <c r="E91">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="F91">
+        <v>0.746</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6">
+      <c r="B92">
+        <v>85</v>
+      </c>
+      <c r="C92" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0.74988889000000003</v>
+      </c>
+      <c r="E92">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="F92">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6">
+      <c r="B93">
+        <v>86</v>
+      </c>
+      <c r="C93" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0.75788889000000004</v>
+      </c>
+      <c r="E93">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="F93">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6">
+      <c r="B94">
+        <v>87</v>
+      </c>
+      <c r="C94" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0.76355556000000002</v>
+      </c>
+      <c r="E94">
+        <v>0.72</v>
+      </c>
+      <c r="F94">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6">
+      <c r="B95">
+        <v>88</v>
+      </c>
+      <c r="C95" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0.76088889000000004</v>
+      </c>
+      <c r="E95">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="F95">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6">
+      <c r="B96">
+        <v>89</v>
+      </c>
+      <c r="C96" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0.75966666999999999</v>
+      </c>
+      <c r="E96">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="F96">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6">
+      <c r="B97">
+        <v>90</v>
+      </c>
+      <c r="C97" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0.76</v>
+      </c>
+      <c r="E97">
+        <v>0.72</v>
+      </c>
+      <c r="F97">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6">
+      <c r="B98">
+        <v>91</v>
+      </c>
+      <c r="C98" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0.76077777999999996</v>
+      </c>
+      <c r="E98">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="F98">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6">
+      <c r="B99">
+        <v>92</v>
+      </c>
+      <c r="C99" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0.76155556000000002</v>
+      </c>
+      <c r="E99">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="F99">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6">
+      <c r="B100">
+        <v>93</v>
+      </c>
+      <c r="C100" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0.76322221999999995</v>
+      </c>
+      <c r="E100">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="F100">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6">
+      <c r="B101">
+        <v>94</v>
+      </c>
+      <c r="C101" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0.76633333000000003</v>
+      </c>
+      <c r="E101">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="F101">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6">
+      <c r="B102">
+        <v>95</v>
+      </c>
+      <c r="C102" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0.76788889000000005</v>
+      </c>
+      <c r="E102">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="F102">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6">
+      <c r="B103">
+        <v>96</v>
+      </c>
+      <c r="C103" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0.77266667</v>
+      </c>
+      <c r="E103">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="F103">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6">
+      <c r="B104">
+        <v>97</v>
+      </c>
+      <c r="C104" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0.78166667000000001</v>
+      </c>
+      <c r="E104">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="F104">
+        <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6">
+      <c r="B105">
+        <v>98</v>
+      </c>
+      <c r="C105" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0.79088888999999996</v>
+      </c>
+      <c r="E105">
+        <v>0.745</v>
+      </c>
+      <c r="F105">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6">
+      <c r="B106">
+        <v>99</v>
+      </c>
+      <c r="C106" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0.79477777999999999</v>
+      </c>
+      <c r="E106">
+        <v>0.749</v>
+      </c>
+      <c r="F106">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6">
+      <c r="B107">
+        <v>100</v>
+      </c>
+      <c r="C107" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0.79533332999999995</v>
+      </c>
+      <c r="E107">
+        <v>0.749</v>
+      </c>
+      <c r="F107">
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:J79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:F79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.10077778</v>
+      </c>
+      <c r="E9">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.10077778</v>
+      </c>
+      <c r="E10">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.10077778</v>
+      </c>
+      <c r="E11">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.10077778</v>
+      </c>
+      <c r="E12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.10077778</v>
+      </c>
+      <c r="E13">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.10077778</v>
+      </c>
+      <c r="E14">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.10077778</v>
+      </c>
+      <c r="E15">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.105</v>
+      </c>
+      <c r="F16">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.105</v>
+      </c>
+      <c r="F17">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.105</v>
+      </c>
+      <c r="F18">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.105</v>
+      </c>
+      <c r="F19">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.105</v>
+      </c>
+      <c r="F20">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.105</v>
+      </c>
+      <c r="F21">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.105</v>
+      </c>
+      <c r="F22">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.105</v>
+      </c>
+      <c r="F23">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.105</v>
+      </c>
+      <c r="F24">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E25">
+        <v>0.105</v>
+      </c>
+      <c r="F25">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.105</v>
+      </c>
+      <c r="F26">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.105</v>
+      </c>
+      <c r="F27">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.105</v>
+      </c>
+      <c r="F28">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E29">
+        <v>0.105</v>
+      </c>
+      <c r="F29">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.105</v>
+      </c>
+      <c r="F30">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.105</v>
+      </c>
+      <c r="F31">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E32">
+        <v>0.105</v>
+      </c>
+      <c r="F32">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E33">
+        <v>0.105</v>
+      </c>
+      <c r="F33">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E34">
+        <v>0.105</v>
+      </c>
+      <c r="F34">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.105</v>
+      </c>
+      <c r="F35">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E36">
+        <v>0.105</v>
+      </c>
+      <c r="F36">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>9.922222E-2</v>
+      </c>
+      <c r="E37">
+        <v>0.105</v>
+      </c>
+      <c r="F37">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0.21211110999999999</v>
+      </c>
+      <c r="E38">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F38">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0.20877778</v>
+      </c>
+      <c r="E39">
+        <v>0.19</v>
+      </c>
+      <c r="F39">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.24611110999999999</v>
+      </c>
+      <c r="E40">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F40">
+        <v>0.24199999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41">
+        <v>33</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="E41">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="F41">
+        <v>0.316</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0.32766666999999999</v>
+      </c>
+      <c r="E42">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="F42">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43">
+        <v>35</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0.36622221999999999</v>
+      </c>
+      <c r="E43">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="F43">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.39411110999999999</v>
+      </c>
+      <c r="E44">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="F44">
+        <v>0.40899999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.43322221999999999</v>
+      </c>
+      <c r="E45">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="F45">
+        <v>0.45600000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0.52222221999999996</v>
+      </c>
+      <c r="E46">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F46">
+        <v>0.56599999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0.62588889000000003</v>
+      </c>
+      <c r="E47">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="F47">
+        <v>0.66200000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0.69377778000000001</v>
+      </c>
+      <c r="E48">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="F48">
+        <v>0.73499999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0.80166667000000003</v>
+      </c>
+      <c r="E49">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="F49">
+        <v>0.83299999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0.85266666999999996</v>
+      </c>
+      <c r="E50">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F50">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51">
+        <v>43</v>
+      </c>
+      <c r="C51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0.86955556000000001</v>
+      </c>
+      <c r="E51">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="F51">
+        <v>0.89400000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52">
+        <v>44</v>
+      </c>
+      <c r="C52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0.87922222000000005</v>
+      </c>
+      <c r="E52">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="F52">
+        <v>0.90300000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53">
+        <v>45</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.88922221999999995</v>
+      </c>
+      <c r="E53">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="F53">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54">
+        <v>46</v>
+      </c>
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0.89577777999999997</v>
+      </c>
+      <c r="E54">
+        <v>0.874</v>
+      </c>
+      <c r="F54">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0.90155556000000003</v>
+      </c>
+      <c r="E55">
+        <v>0.875</v>
+      </c>
+      <c r="F55">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0.90555556000000004</v>
+      </c>
+      <c r="E56">
+        <v>0.878</v>
+      </c>
+      <c r="F56">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57">
+        <v>49</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0.90744444000000002</v>
+      </c>
+      <c r="E57">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="F57">
+        <v>0.91900000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58">
+        <v>50</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0.91077777999999998</v>
+      </c>
+      <c r="E58">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="F58">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0.91377777999999998</v>
+      </c>
+      <c r="E59">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="F59">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60">
+        <v>52</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0.91466667000000001</v>
+      </c>
+      <c r="E60">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="F60">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="B61">
+        <v>53</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0.91688888999999996</v>
+      </c>
+      <c r="E61">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="F61">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62">
+        <v>54</v>
+      </c>
+      <c r="C62" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0.91888888999999996</v>
+      </c>
+      <c r="E62">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="F62">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0.92</v>
+      </c>
+      <c r="E63">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="F63">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64">
+        <v>56</v>
+      </c>
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0.92033332999999995</v>
+      </c>
+      <c r="E64">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="F64">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65">
+        <v>57</v>
+      </c>
+      <c r="C65" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0.92144444000000003</v>
+      </c>
+      <c r="E65">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="F65">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66">
+        <v>58</v>
+      </c>
+      <c r="C66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0.92244444000000003</v>
+      </c>
+      <c r="E66">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="F66">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67">
+        <v>59</v>
+      </c>
+      <c r="C67" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0.92222221999999998</v>
+      </c>
+      <c r="E67">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="F67">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68">
+        <v>60</v>
+      </c>
+      <c r="C68" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0.92366667000000002</v>
+      </c>
+      <c r="E68">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="F68">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69">
+        <v>61</v>
+      </c>
+      <c r="C69" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0.92488888999999996</v>
+      </c>
+      <c r="E69">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="F69">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70">
+        <v>62</v>
+      </c>
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0.92644444000000004</v>
+      </c>
+      <c r="E70">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="F70">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71">
+        <v>63</v>
+      </c>
+      <c r="C71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0.92788888999999997</v>
+      </c>
+      <c r="E71">
+        <v>0.9</v>
+      </c>
+      <c r="F71">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72">
+        <v>64</v>
+      </c>
+      <c r="C72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0.92877778</v>
+      </c>
+      <c r="E72">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="F72">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73">
+        <v>65</v>
+      </c>
+      <c r="C73" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0.92966667000000003</v>
+      </c>
+      <c r="E73">
+        <v>0.9</v>
+      </c>
+      <c r="F73">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74">
+        <v>66</v>
+      </c>
+      <c r="C74" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.93077778</v>
+      </c>
+      <c r="E74">
+        <v>0.9</v>
+      </c>
+      <c r="F74">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75">
+        <v>67</v>
+      </c>
+      <c r="C75" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0.93144444000000004</v>
+      </c>
+      <c r="E75">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="F75">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76">
+        <v>68</v>
+      </c>
+      <c r="C76" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0.93233332999999996</v>
+      </c>
+      <c r="E76">
+        <v>0.9</v>
+      </c>
+      <c r="F76">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77">
+        <v>69</v>
+      </c>
+      <c r="C77" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0.93288888999999997</v>
+      </c>
+      <c r="E77">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="F77">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78">
+        <v>70</v>
+      </c>
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0.93388888999999997</v>
+      </c>
+      <c r="E78">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="F78">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="B79">
+        <v>71</v>
+      </c>
+      <c r="C79" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="E79">
+        <v>0.9</v>
+      </c>
+      <c r="F79">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>